<commit_message>
aligning ObjTables with SBtab; removing SBtab mode
</commit_message>
<xml_diff>
--- a/examples/parents_children.xlsx
+++ b/examples/parents_children.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13965" activeTab="3"/>
+    <workbookView windowWidth="20295" windowHeight="6945" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -158,9 +158,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="66">
-  <si>
-    <t>!!SBtab TableType='TableOfContents' TableName='Table of contents' Description='Table/model and column/attribute definitions' Date='2019-09-18 13:17:59' SBtabVersion='2.0'</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="65">
+  <si>
+    <t>!!ObjTables TableType='TableOfContents' Description='Table/model and column/attribute definitions' Date='2019-09-18 13:17:59' ObjTablesVersion='2.0'</t>
   </si>
   <si>
     <t>!Table</t>
@@ -178,22 +178,22 @@
     <t>Parent</t>
   </si>
   <si>
-    <t>!!SBtab TableType='Schema' TableName='Table/model and column/attribute definitions' SBtabVersion='2.0'</t>
-  </si>
-  <si>
-    <t>!ComponentName</t>
-  </si>
-  <si>
-    <t>!ComponentType</t>
-  </si>
-  <si>
-    <t>!IsPartOf</t>
+    <t>!!ObjTables TableType='Schema' Description='Table/model and column/attribute definitions' ObjTablesVersion='0.0.8'</t>
+  </si>
+  <si>
+    <t>!Name</t>
+  </si>
+  <si>
+    <t>!Type</t>
+  </si>
+  <si>
+    <t>!Parent</t>
   </si>
   <si>
     <t>!Format</t>
   </si>
   <si>
-    <t>Table</t>
+    <t>Model</t>
   </si>
   <si>
     <t>column</t>
@@ -202,16 +202,16 @@
     <t>Id</t>
   </si>
   <si>
-    <t>Column</t>
-  </si>
-  <si>
-    <t>string(unique=True, primary=True)</t>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>String(unique=True, primary=True)</t>
   </si>
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>string</t>
+    <t>String</t>
   </si>
   <si>
     <t>row</t>
@@ -220,19 +220,19 @@
     <t>Gender</t>
   </si>
   <si>
-    <t>enum(['female', 'male'])</t>
+    <t>Enum(['female', 'male'])</t>
   </si>
   <si>
     <t>Parents</t>
   </si>
   <si>
-    <t>manyToMany('Parent', related_name='children')</t>
+    <t>ManyToMany('Parent', related_name='children')</t>
   </si>
   <si>
     <t>FavoriteVideoGame</t>
   </si>
   <si>
-    <t>manyToOne('Game', related_name='children')</t>
+    <t>ManyToOne('Game', related_name='children')</t>
   </si>
   <si>
     <t>Game</t>
@@ -247,10 +247,10 @@
     <t>Year</t>
   </si>
   <si>
-    <t>integer</t>
-  </si>
-  <si>
-    <t>!!SBtab TableType='Data' TableID='Parent' TableName='Parent' Date='2019-09-18 13:17:59' SBtabVersion='2.0'</t>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>!!ObjTables TableType='Data' ModelId='Parent' ModelName='Parent' Date='2019-09-18 13:17:59' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Id</t>
@@ -268,9 +268,6 @@
     <t>richard_roe</t>
   </si>
   <si>
-    <t>!Name</t>
-  </si>
-  <si>
     <t>Jane Doe</t>
   </si>
   <si>
@@ -283,7 +280,7 @@
     <t>Richard Roe</t>
   </si>
   <si>
-    <t>!!SBtab TableType='Data' TableID='Child' TableName='Child' Date='2019-09-18 13:17:59' SBtabVersion='2.0'</t>
+    <t>!!ObjTables TableType='Data' ModelId='Child' ModelName='Child' Date='2019-09-18 13:17:59' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!FavoriteVideoGame</t>
@@ -363,10 +360,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -390,6 +387,52 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -397,8 +440,69 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -412,67 +516,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -482,57 +525,11 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="37">
     <fill>
@@ -567,187 +564,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -761,17 +758,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -806,15 +806,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -832,9 +823,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -848,161 +841,165 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1446,7 +1443,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelCol="3"/>
@@ -1663,12 +1660,12 @@
   <sheetPr/>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1" outlineLevelRow="2" outlineLevelCol="4"/>
@@ -1705,19 +1702,19 @@
     </row>
     <row r="3" customHeight="1" spans="1:5">
       <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1741,7 +1738,7 @@
   <sheetPr/>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1755,7 +1752,7 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1770,13 +1767,13 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:7">
@@ -1784,42 +1781,42 @@
         <v>31</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:7">
       <c r="A4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="G4" s="4">
         <v>1986</v>
@@ -1827,22 +1824,22 @@
     </row>
     <row r="5" customHeight="1" spans="1:7">
       <c r="A5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="F5" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G5" s="4">
         <v>1985</v>
@@ -1850,22 +1847,22 @@
     </row>
     <row r="6" customHeight="1" spans="1:7">
       <c r="A6" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="G6" s="4">
         <v>1991</v>
@@ -1873,22 +1870,22 @@
     </row>
     <row r="7" customHeight="1" spans="1:7">
       <c r="A7" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="G7" s="4">
         <v>1989</v>
@@ -1903,16 +1900,16 @@
     <mergeCell ref="E2:G2"/>
   </mergeCells>
   <dataValidations count="7">
+    <dataValidation type="whole" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="!Year" error="Value must be an integer." promptTitle="!Year" prompt="Enter an integer." sqref="G4:G7" errorStyle="warning">
+      <formula1>-32768</formula1>
+      <formula2>32767</formula2>
+    </dataValidation>
     <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="!Publisher" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="!Publisher" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="F4:F7" errorStyle="warning">
       <formula1>255</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="!Parents" error="Value must be a comma-separated list of values from &quot;!Parent:1&quot; or blank." promptTitle="!Parents" prompt="Enter a comma-separated list of values from &quot;!Parent:1&quot; or blank." sqref="D4:D7" errorStyle="warning"/>
     <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="!Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="!Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." sqref="E4:E7" errorStyle="warning">
       <formula1>255</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="!Parents" error="Value must be a comma-separated list of values from &quot;!Parent:1&quot; or blank." promptTitle="!Parents" prompt="Enter a comma-separated list of values from &quot;!Parent:1&quot; or blank." sqref="D4:D7" errorStyle="warning"/>
-    <dataValidation type="whole" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="!Year" error="Value must be an integer." promptTitle="!Year" prompt="Enter an integer." sqref="G4:G7" errorStyle="warning">
-      <formula1>-32768</formula1>
-      <formula2>32767</formula2>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="!Gender" error="Value must be one of &quot;female&quot;, &quot;male&quot;." promptTitle="!Gender" prompt="Select one of &quot;female&quot;, &quot;male&quot;." sqref="C4:C7" errorStyle="warning">
       <formula1>"female,male"</formula1>

</xml_diff>